<commit_message>
Lesson 10 homework added
</commit_message>
<xml_diff>
--- a/09/ClassWork/О Эн квадрат.xlsx
+++ b/09/ClassWork/О Эн квадрат.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\it-nordic-cs\09\ClassWork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\almis\Рабочий стол\ItNordic\it-nordic-cs\09\ClassWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AAEBE1-93A4-4F34-B274-FA876CABDFF6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,7 +90,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -140,6 +140,21 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="41275" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Лист1!$A$1:$A$10</c:f>
@@ -216,6 +231,106 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-235D-4FC3-AE84-2FC925331838}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$1:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$C$1:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>372</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1478</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6887</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26633</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>96630</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>384116</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1502695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F5E3-4683-9065-25E42F8279F5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -234,7 +349,6 @@
         <c:axId val="421452776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="200000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -960,20 +1074,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvPr id="2" name="Диаграмма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1253,24 +1373,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1000</v>
       </c>
       <c r="B1">
         <v>3</v>
       </c>
+      <c r="C1">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1*2</f>
         <v>2000</v>
@@ -1278,8 +1401,11 @@
       <c r="B2">
         <v>14</v>
       </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A10" si="0">A2*2</f>
         <v>4000</v>
@@ -1287,8 +1413,11 @@
       <c r="B3">
         <v>66</v>
       </c>
+      <c r="C3">
+        <v>82</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1296,8 +1425,11 @@
       <c r="B4">
         <v>252</v>
       </c>
+      <c r="C4">
+        <v>372</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>16000</v>
@@ -1305,8 +1437,11 @@
       <c r="B5">
         <v>998</v>
       </c>
+      <c r="C5">
+        <v>1478</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>32000</v>
@@ -1314,8 +1449,11 @@
       <c r="B6">
         <v>4066</v>
       </c>
+      <c r="C6">
+        <v>6887</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>64000</v>
@@ -1323,8 +1461,11 @@
       <c r="B7">
         <v>16211</v>
       </c>
+      <c r="C7">
+        <v>26633</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>128000</v>
@@ -1332,17 +1473,26 @@
       <c r="B8">
         <v>67934</v>
       </c>
+      <c r="C8">
+        <v>96630</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>256000</v>
       </c>
+      <c r="C9">
+        <v>384116</v>
+      </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>512000</v>
+      </c>
+      <c r="C10">
+        <v>1502695</v>
       </c>
     </row>
   </sheetData>

</xml_diff>